<commit_message>
User description with video and cover
</commit_message>
<xml_diff>
--- a/contact-todo.xlsx
+++ b/contact-todo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>User Profile</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Boutton messages avec compteur et liste des messages reçus</t>
+  </si>
+  <si>
+    <t>OK</t>
   </si>
 </sst>
 </file>
@@ -374,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -385,7 +388,7 @@
     <col min="2" max="2" width="87.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -393,47 +396,50 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Use video for profile photo
</commit_message>
<xml_diff>
--- a/contact-todo.xlsx
+++ b/contact-todo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>User Profile</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>OK</t>
+  </si>
+  <si>
+    <t>Afficher une vidéo de profil au lieu d'une photo</t>
   </si>
 </sst>
 </file>
@@ -377,10 +380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,52 +398,60 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
correct bug add animation to contact list
</commit_message>
<xml_diff>
--- a/contact-todo.xlsx
+++ b/contact-todo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>User Profile</t>
   </si>
@@ -33,9 +33,6 @@
   </si>
   <si>
     <t>Partager le contact (Partage réseaux sociaux)</t>
-  </si>
-  <si>
-    <t>Partager une vidéo (2j max)</t>
   </si>
   <si>
     <t>Retirer un contact</t>
@@ -380,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,20 +396,20 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -427,7 +424,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -448,11 +445,6 @@
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
browse contact in anymous mode
</commit_message>
<xml_diff>
--- a/contact-todo.xlsx
+++ b/contact-todo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>User Profile</t>
   </si>
@@ -380,7 +380,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -403,6 +403,9 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">

</xml_diff>

<commit_message>
Share contact view profile
</commit_message>
<xml_diff>
--- a/contact-todo.xlsx
+++ b/contact-todo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>User Profile</t>
   </si>
@@ -380,7 +380,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,6 +419,9 @@
       <c r="B4" t="s">
         <v>2</v>
       </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">

</xml_diff>

<commit_message>
Display link button only if the user is authenticated and if he isn't on it own profile
</commit_message>
<xml_diff>
--- a/contact-todo.xlsx
+++ b/contact-todo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>User Profile</t>
   </si>
@@ -380,7 +380,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,6 +427,9 @@
       <c r="B5" t="s">
         <v>3</v>
       </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">

</xml_diff>

<commit_message>
size photo in contact suggestion list on mobile device
</commit_message>
<xml_diff>
--- a/contact-todo.xlsx
+++ b/contact-todo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>User Profile</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>Afficher une vidéo de profil au lieu d'une photo</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bug : taille d'image </t>
   </si>
 </sst>
 </file>
@@ -377,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -388,7 +394,7 @@
     <col min="2" max="2" width="87.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -399,15 +405,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -415,7 +424,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -423,7 +432,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -431,29 +440,44 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>